<commit_message>
fix: some minor fixes
</commit_message>
<xml_diff>
--- a/VerificationMatrix.xlsx
+++ b/VerificationMatrix.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8632D033-5783-4DF6-8550-DAF916FDF8D6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08C83615-6965-4DF6-9670-A1BE51F6B0F3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -46,12 +46,6 @@
     <t>GenFigScVsBulk.R</t>
   </si>
   <si>
-    <t>GenFigSourcesOfVar.R</t>
-  </si>
-  <si>
-    <t>RandomForestFineGrainedVarImp.R</t>
-  </si>
-  <si>
     <t>RandomForestGroupVarImp.R</t>
   </si>
   <si>
@@ -128,6 +122,12 @@
   </si>
   <si>
     <t>Figure generation code. The graphs look reasonable and the data presented is as expected.</t>
+  </si>
+  <si>
+    <t>GenFigSourcesOfVarPairWise.R</t>
+  </si>
+  <si>
+    <t>Manually checked that the number of technical replicate pairs per lab was correct. The results in all looks as expected. No further tests were deemed necessary.</t>
   </si>
 </sst>
 </file>
@@ -460,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,7 +474,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -485,7 +485,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -493,7 +493,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -501,7 +501,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -509,63 +509,63 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -573,23 +573,23 @@
         <v>5</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -597,7 +597,7 @@
         <v>6</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -605,25 +605,24 @@
         <v>7</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="2"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B19" s="2"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>10</v>
-      </c>
       <c r="B20" s="2"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -637,9 +636,6 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
upd: Update verification matrix
</commit_message>
<xml_diff>
--- a/VerificationMatrix.xlsx
+++ b/VerificationMatrix.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08C83615-6965-4DF6-9670-A1BE51F6B0F3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED667B13-3BA1-0245-B395-F58AD97AF9BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Verification/validation</t>
   </si>
@@ -128,6 +128,15 @@
   </si>
   <si>
     <t>Manually checked that the number of technical replicate pairs per lab was correct. The results in all looks as expected. No further tests were deemed necessary.</t>
+  </si>
+  <si>
+    <t>RandomForestFunc.R</t>
+  </si>
+  <si>
+    <t>Each aspect of the RF forest estimation was checked during construction of the function. Construction of the CART trees is done with a package function from randomForestSRC. Estimation of OOB error and variable importance are implemented in a standard fashion and results have been checked to show expected behaviour.</t>
+  </si>
+  <si>
+    <t>Data loading and data transformations were checked manually for correctness. Result look reasonable, especially compared to pairwise method in GenFigSourcesOfVarPairWise.R.</t>
   </si>
 </sst>
 </file>
@@ -462,17 +471,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.7109375" customWidth="1"/>
-    <col min="2" max="2" width="94.7109375" customWidth="1"/>
+    <col min="1" max="1" width="36.6640625" customWidth="1"/>
+    <col min="2" max="2" width="94.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -480,7 +489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -488,7 +497,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -496,7 +505,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -504,7 +513,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -512,7 +521,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -520,7 +529,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
@@ -528,7 +537,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
@@ -536,7 +545,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
@@ -544,7 +553,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>21</v>
       </c>
@@ -552,7 +561,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>23</v>
       </c>
@@ -560,7 +569,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>25</v>
       </c>
@@ -568,7 +577,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -576,7 +585,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>28</v>
       </c>
@@ -584,7 +593,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>30</v>
       </c>
@@ -592,7 +601,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -600,7 +609,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -608,7 +617,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -616,25 +625,32 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="2"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="2"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B21" s="2"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B22" s="2"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B23" s="2"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B24" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Added supplementary graph for quantile normalized data (Fig S3, similar to fig 6)
</commit_message>
<xml_diff>
--- a/VerificationMatrix.xlsx
+++ b/VerificationMatrix.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED667B13-3BA1-0245-B395-F58AD97AF9BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC20D15-32E4-42C4-B748-B2AD500379FC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <t>Verification/validation</t>
   </si>
@@ -137,6 +137,18 @@
   </si>
   <si>
     <t>Data loading and data transformations were checked manually for correctness. Result look reasonable, especially compared to pairwise method in GenFigSourcesOfVarPairWise.R.</t>
+  </si>
+  <si>
+    <t>GenerateScVsBulkDataQuantile.R</t>
+  </si>
+  <si>
+    <t>GenFigScVsBulkQuantile.R</t>
+  </si>
+  <si>
+    <t>This code is copied from GenFigScVsBulk.R and is very similar. A manual check that we loaded the right file was done, and the results look reasonable and a bit different from the TMM-normalized data. No other verification was deemed necessary.</t>
+  </si>
+  <si>
+    <t>TC004, found at the end of the code - the rest of the code is copied from GenerateScVsBulkData.R and is therefore tested as part of those tests. The data looks quantile normalized. No other verification was deemed necessary.</t>
   </si>
 </sst>
 </file>
@@ -469,19 +481,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.6640625" customWidth="1"/>
-    <col min="2" max="2" width="94.6640625" customWidth="1"/>
+    <col min="1" max="1" width="36.7109375" customWidth="1"/>
+    <col min="2" max="2" width="94.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -489,7 +501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -497,7 +509,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -505,7 +517,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -513,7 +525,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -521,7 +533,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -529,7 +541,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
@@ -537,7 +549,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
@@ -545,7 +557,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
@@ -553,7 +565,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>21</v>
       </c>
@@ -561,7 +573,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>23</v>
       </c>
@@ -569,7 +581,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>25</v>
       </c>
@@ -577,7 +589,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -585,7 +597,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>28</v>
       </c>
@@ -593,7 +605,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>30</v>
       </c>
@@ -601,57 +613,73 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>6</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>7</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="48" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="21" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="22" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B21" s="2"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B22" s="2"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
test: Filled in the verification matrix with some new functions.
</commit_message>
<xml_diff>
--- a/VerificationMatrix.xlsx
+++ b/VerificationMatrix.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC20D15-32E4-42C4-B748-B2AD500379FC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B681FB-EA56-40D8-8FA6-F530C4946C96}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -46,9 +46,6 @@
     <t>GenFigScVsBulk.R</t>
   </si>
   <si>
-    <t>RandomForestGroupVarImp.R</t>
-  </si>
-  <si>
     <t>It is difficult to verify this code with test cases. The code has been reviewed, and the output looks as expected in Fig 2: The data in general cluster on dataset, but still separate on cell type. The conclusion is that this looks reasonable and that no further testing is required.</t>
   </si>
   <si>
@@ -124,21 +121,6 @@
     <t>Figure generation code. The graphs look reasonable and the data presented is as expected.</t>
   </si>
   <si>
-    <t>GenFigSourcesOfVarPairWise.R</t>
-  </si>
-  <si>
-    <t>Manually checked that the number of technical replicate pairs per lab was correct. The results in all looks as expected. No further tests were deemed necessary.</t>
-  </si>
-  <si>
-    <t>RandomForestFunc.R</t>
-  </si>
-  <si>
-    <t>Each aspect of the RF forest estimation was checked during construction of the function. Construction of the CART trees is done with a package function from randomForestSRC. Estimation of OOB error and variable importance are implemented in a standard fashion and results have been checked to show expected behaviour.</t>
-  </si>
-  <si>
-    <t>Data loading and data transformations were checked manually for correctness. Result look reasonable, especially compared to pairwise method in GenFigSourcesOfVarPairWise.R.</t>
-  </si>
-  <si>
     <t>GenerateScVsBulkDataQuantile.R</t>
   </si>
   <si>
@@ -149,6 +131,24 @@
   </si>
   <si>
     <t>TC004, found at the end of the code - the rest of the code is copied from GenerateScVsBulkData.R and is therefore tested as part of those tests. The data looks quantile normalized. No other verification was deemed necessary.</t>
+  </si>
+  <si>
+    <t>GenFigSourcesOfVarVP.R</t>
+  </si>
+  <si>
+    <t>In general, there is not much logic. There is a risk of mixing samples up - it is however unlikely that an unmatchning design matrix and data matrix are used together - they must have the same number of samples. For selection of LM22S, the results look as expected, with a higher explained variance for cell subType. For variance explained vs gene expression, the residuals look as expected, so it most likely works. Outlier check: The code is fairly straight forward, and the results look somewhat as expected.</t>
+  </si>
+  <si>
+    <t>GenDeconvData.R</t>
+  </si>
+  <si>
+    <t>The code has not been formally verified, but it is fairly simple and generates the expected output. The end results of the deconvolution also very much looks as expected, with the internal lab 4 having the least relative error, and so forth.</t>
+  </si>
+  <si>
+    <t>GenFigDeconv.R</t>
+  </si>
+  <si>
+    <t>The code has not been formally verified, but it is fairly simple and generates the expected plots. The results of the deconvolution also very much looks as expected, with the internal lab 4 having the least relative error, and so forth.</t>
   </si>
 </sst>
 </file>
@@ -483,8 +483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,7 +495,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -506,7 +506,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -514,7 +514,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -522,7 +522,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -530,63 +530,63 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -594,31 +594,31 @@
         <v>5</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -626,7 +626,7 @@
         <v>6</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -634,39 +634,39 @@
         <v>7</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="2" t="s">
+    </row>
+    <row r="22" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>8</v>
-      </c>
       <c r="B22" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>